<commit_message>
+ Comment in ukrainian, fixes and profile fixes. To do: Data cleaning, dashboards Probably history and projects
</commit_message>
<xml_diff>
--- a/web/backend/files test/data cleaning/dirty_data_example_1.xlsx
+++ b/web/backend/files test/data cleaning/dirty_data_example_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\4 Year\Diploma\version1\web\backend\files test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\4 Year\Diploma\version1\web\backend\files test\data cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FA5D6F-F350-407A-9E4F-66EC0A6DEF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EA892E-F0F3-422F-BAAD-4763D5ACDACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="2985" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4665" yWindow="4665" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -116,6 +116,21 @@
   </si>
   <si>
     <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>some1</t>
+  </si>
+  <si>
+    <t>some23</t>
+  </si>
+  <si>
+    <t>sefse</t>
+  </si>
+  <si>
+    <t>ffvhthg</t>
+  </si>
+  <si>
+    <t>eswwfd</t>
   </si>
 </sst>
 </file>
@@ -147,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -170,13 +185,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -483,15 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,8 +536,23 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -525,7 +569,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -542,7 +586,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -556,7 +600,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -573,7 +617,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -590,7 +634,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -607,7 +651,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -624,7 +668,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -638,7 +682,7 @@
         <v>65000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -652,7 +696,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Data Cleaning ready To do: Dashboards
</commit_message>
<xml_diff>
--- a/web/backend/files test/data cleaning/dirty_data_example_1.xlsx
+++ b/web/backend/files test/data cleaning/dirty_data_example_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\4 Year\Diploma\version1\web\backend\files test\data cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EA892E-F0F3-422F-BAAD-4763D5ACDACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28CAB3B-D80B-4364-9463-D304BAD5ED7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4665" yWindow="4665" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -116,21 +116,6 @@
   </si>
   <si>
     <t xml:space="preserve">     </t>
-  </si>
-  <si>
-    <t>some1</t>
-  </si>
-  <si>
-    <t>some23</t>
-  </si>
-  <si>
-    <t>sefse</t>
-  </si>
-  <si>
-    <t>ffvhthg</t>
-  </si>
-  <si>
-    <t>eswwfd</t>
   </si>
 </sst>
 </file>
@@ -205,7 +190,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -515,7 +500,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,21 +521,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>